<commit_message>
timerecording update issue numbers
</commit_message>
<xml_diff>
--- a/Sprint2 5Schuhljahr.xlsx
+++ b/Sprint2 5Schuhljahr.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\4Schuljahr\syp\Projekt\multiflexlbkv\multiflexlbkv\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C68AEB7B-201E-4C7C-B8A8-57785AA92062}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1868932C-7458-4B00-9277-8103DC1E07E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12252" activeTab="1" xr2:uid="{DE4AF553-B22C-4BF0-B016-1373DC96BC61}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="25">
   <si>
     <t>Zeiterfassung 5 Schuljahr</t>
   </si>
@@ -109,6 +109,9 @@
   </si>
   <si>
     <t>Logic für das einfügen #44</t>
+  </si>
+  <si>
+    <t>Datenbank Checksum #43</t>
   </si>
 </sst>
 </file>
@@ -1392,7 +1395,7 @@
   <dimension ref="A1:AC29"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1718,12 +1721,12 @@
         <v>0.3125</v>
       </c>
       <c r="D9" s="54">
-        <v>0.66666666666666663</v>
+        <v>0.58333333333333337</v>
       </c>
       <c r="E9" s="58"/>
       <c r="F9" s="54">
         <f t="shared" ref="F9:F17" si="0">SUM(D9-C9)</f>
-        <v>0.35416666666666663</v>
+        <v>0.27083333333333337</v>
       </c>
       <c r="G9" s="18" t="s">
         <v>15</v>
@@ -1831,16 +1834,18 @@
         <v>0.39583333333333331</v>
       </c>
       <c r="D11" s="54">
-        <v>0.66666666666666663</v>
+        <v>0.75</v>
       </c>
       <c r="E11" s="54">
         <v>2.0833333333333332E-2</v>
       </c>
       <c r="F11" s="54">
         <f>SUM(D11-C11-E11)</f>
-        <v>0.24999999999999997</v>
-      </c>
-      <c r="G11" s="28"/>
+        <v>0.33333333333333337</v>
+      </c>
+      <c r="G11" s="28" t="s">
+        <v>24</v>
+      </c>
       <c r="H11" s="29"/>
       <c r="I11" s="30"/>
       <c r="J11" s="21" t="s">
@@ -1988,7 +1993,7 @@
       <c r="E14" s="62"/>
       <c r="F14" s="61">
         <f>SUM(F11+F9)</f>
-        <v>0.60416666666666663</v>
+        <v>0.60416666666666674</v>
       </c>
       <c r="G14" s="49"/>
       <c r="H14" s="49"/>
@@ -2233,11 +2238,10 @@
       <c r="E29" s="48"/>
     </row>
   </sheetData>
-  <mergeCells count="50">
+  <mergeCells count="51">
     <mergeCell ref="N9:N10"/>
     <mergeCell ref="W12:W13"/>
     <mergeCell ref="W9:W10"/>
-    <mergeCell ref="G10:I11"/>
     <mergeCell ref="D9:D10"/>
     <mergeCell ref="C9:C10"/>
     <mergeCell ref="B9:B10"/>
@@ -2267,11 +2271,13 @@
     <mergeCell ref="G13:I13"/>
     <mergeCell ref="P13:R13"/>
     <mergeCell ref="Y14:AA14"/>
+    <mergeCell ref="G11:I11"/>
     <mergeCell ref="G12:I12"/>
     <mergeCell ref="P11:R12"/>
     <mergeCell ref="O11:O12"/>
     <mergeCell ref="N11:N12"/>
     <mergeCell ref="G9:I9"/>
+    <mergeCell ref="G10:I10"/>
     <mergeCell ref="P9:R10"/>
     <mergeCell ref="Y9:AA10"/>
     <mergeCell ref="T9:T10"/>

</xml_diff>